<commit_message>
Commit 2019-04-26 kl. 17:47
</commit_message>
<xml_diff>
--- a/Work/Fixzone/Tasks/Task1/Task11_Day13_Date190417_Review of collection sql queries for ShopDirect/SD Comms - Expected Output.xlsx
+++ b/Work/Fixzone/Tasks/Task1/Task11_Day13_Date190417_Review of collection sql queries for ShopDirect/SD Comms - Expected Output.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1470" windowWidth="18300" windowHeight="5880"/>
+    <workbookView xWindow="1920" yWindow="1470" windowWidth="18300" windowHeight="5880" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
   <si>
     <t>comms no.</t>
   </si>
@@ -181,6 +180,111 @@
   </si>
   <si>
     <t>L = Littlewoods</t>
+  </si>
+  <si>
+    <t>Courier Dispatch - Very</t>
+  </si>
+  <si>
+    <t>Courier at Depot - V RPG</t>
+  </si>
+  <si>
+    <t>Loan TV Dispatch - Very</t>
+  </si>
+  <si>
+    <t>Claim Closed - VERY</t>
+  </si>
+  <si>
+    <t>BER RPG - VERY</t>
+  </si>
+  <si>
+    <t>Courier Booked SMS Very</t>
+  </si>
+  <si>
+    <t>Failed Appt - Very SMS</t>
+  </si>
+  <si>
+    <t>B2B Repair - VERY RPG</t>
+  </si>
+  <si>
+    <t>New SG - Littlewoods</t>
+  </si>
+  <si>
+    <t>Survey - Very RPG/MPI</t>
+  </si>
+  <si>
+    <t>Appointment Reminder Littlewoods</t>
+  </si>
+  <si>
+    <t>Courier Booked LW</t>
+  </si>
+  <si>
+    <t>Courier Repair Complete - LW</t>
+  </si>
+  <si>
+    <t>Courier Despatch - LW</t>
+  </si>
+  <si>
+    <t>Courier Booked SMS LW</t>
+  </si>
+  <si>
+    <t>Appointment Cancelled LW</t>
+  </si>
+  <si>
+    <t>Failed Appointment - LW</t>
+  </si>
+  <si>
+    <t>Courier at Depot - LW</t>
+  </si>
+  <si>
+    <t>Courier at Depot - LW RPG</t>
+  </si>
+  <si>
+    <t>Claim Closed - LW RGP/MPI</t>
+  </si>
+  <si>
+    <t>Delayed Appointment - LW</t>
+  </si>
+  <si>
+    <t>Job Complete - LW</t>
+  </si>
+  <si>
+    <t>B2B Repair - LW</t>
+  </si>
+  <si>
+    <t>B2B Repair - LW RPG</t>
+  </si>
+  <si>
+    <t>Claim Closed - LW</t>
+  </si>
+  <si>
+    <t>Delayed Appointment - SMS</t>
+  </si>
+  <si>
+    <t>BER</t>
+  </si>
+  <si>
+    <t>Courier at Depot - SMS</t>
+  </si>
+  <si>
+    <t>Courier Despatched - SMS</t>
+  </si>
+  <si>
+    <t>Courier Repair Complete- SMS</t>
+  </si>
+  <si>
+    <t>B2BSMS</t>
+  </si>
+  <si>
+    <t>ApologyV</t>
+  </si>
+  <si>
+    <t>ApologyLW</t>
+  </si>
+  <si>
+    <t>Delayed-SMS</t>
+  </si>
+  <si>
+    <t>Annual health check very- extension</t>
   </si>
 </sst>
 </file>
@@ -659,7 +763,9 @@
   </sheetPr>
   <dimension ref="A2:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1195,24 +1301,262 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B4:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17">
+        <v>54</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>63</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 2019-04-28 kl. 23:52
</commit_message>
<xml_diff>
--- a/Work/Fixzone/Tasks/Task1/Task11_Day13_Date190417_Review of collection sql queries for ShopDirect/SD Comms - Expected Output.xlsx
+++ b/Work/Fixzone/Tasks/Task1/Task11_Day13_Date190417_Review of collection sql queries for ShopDirect/SD Comms - Expected Output.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_cjonasl\Leander\Work\Fixzone\Tasks\Task1\Task11_Day13_Date190417_Review of collection sql queries for ShopDirect\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72AFBD2-ADE9-4691-8649-CCDD6C8A9FD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1470" windowWidth="18300" windowHeight="5880" activeTab="1"/>
+    <workbookView minimized="1" xWindow="4410" yWindow="585" windowWidth="7500" windowHeight="10335" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -290,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -327,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +360,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -456,6 +468,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -466,6 +479,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -514,7 +530,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,9 +563,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -582,6 +615,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -757,7 +807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1300,8 +1350,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B4:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1310,49 +1360,58 @@
     <col min="3" max="3" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="14">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="14">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>59</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="14">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>31</v>
       </c>
@@ -1366,7 +1425,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>32</v>
       </c>
@@ -1380,7 +1439,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>33</v>
       </c>
@@ -1394,7 +1453,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>37</v>
       </c>
@@ -1408,7 +1467,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>39</v>
       </c>
@@ -1422,7 +1481,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>48</v>
       </c>
@@ -1436,7 +1495,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>51</v>
       </c>
@@ -1450,7 +1509,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>56</v>
       </c>
@@ -1464,7 +1523,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>60</v>
       </c>
@@ -1478,7 +1537,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Commit 2019-04-29 kl. 17:32
</commit_message>
<xml_diff>
--- a/Work/Fixzone/Tasks/Task1/Task11_Day13_Date190417_Review of collection sql queries for ShopDirect/SD Comms - Expected Output.xlsx
+++ b/Work/Fixzone/Tasks/Task1/Task11_Day13_Date190417_Review of collection sql queries for ShopDirect/SD Comms - Expected Output.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_cjonasl\Leander\Work\Fixzone\Tasks\Task1\Task11_Day13_Date190417_Review of collection sql queries for ShopDirect\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72AFBD2-ADE9-4691-8649-CCDD6C8A9FD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4410" yWindow="585" windowWidth="7500" windowHeight="10335" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="585" windowWidth="7500" windowHeight="10335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="95">
   <si>
     <t>comms no.</t>
   </si>
@@ -291,12 +285,27 @@
   </si>
   <si>
     <t>Annual health check very- extension</t>
+  </si>
+  <si>
+    <t>Appointment Reminder Very</t>
+  </si>
+  <si>
+    <t>Survey - Very</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>Courier Repair Complete - Very</t>
+  </si>
+  <si>
+    <t>B2B Repair - Very</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -333,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +375,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,6 +484,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -530,7 +546,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -563,26 +579,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,23 +614,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -807,7 +789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -885,7 +867,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -941,7 +923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>3</v>
       </c>
@@ -969,7 +951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>4</v>
       </c>
@@ -997,7 +979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -1350,8 +1332,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B4:I21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1361,10 +1343,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="B4" s="14">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="14" t="s">
         <v>57</v>
       </c>
       <c r="E4" s="14">
@@ -1378,10 +1360,10 @@
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="14">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="14" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="14">
@@ -1395,11 +1377,11 @@
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>59</v>
+      <c r="B6" s="14">
+        <v>56</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="E6" s="14">
         <v>29</v>
@@ -1412,208 +1394,318 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="E7" s="14">
+        <v>41</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="15">
+        <v>27</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="14">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E7">
+      <c r="E9" s="14">
+        <v>43</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
+        <v>32</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="14">
+        <v>42</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="14">
+        <v>39</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="14">
+        <v>45</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="14">
+        <v>48</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="14">
+        <v>46</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="14">
+        <v>51</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="14">
+        <v>47</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="14">
+        <v>60</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="14">
+        <v>50</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="14">
+        <v>59</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="14">
+        <v>61</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="14">
+        <v>62</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="14">
+        <v>63</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E23" s="14">
+        <v>33</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="14">
+        <v>11</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E26" s="14">
+        <v>37</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E28" s="14">
+        <v>21</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E29" s="14">
         <v>35</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F29" s="14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8">
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E33" s="14">
+        <v>19</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34" s="14">
         <v>40</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F34" s="14" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9">
-        <v>43</v>
-      </c>
-      <c r="F9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10">
-        <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12">
-        <v>45</v>
-      </c>
-      <c r="F12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13">
-        <v>46</v>
-      </c>
-      <c r="F13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>56</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14">
-        <v>47</v>
-      </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>60</v>
-      </c>
-      <c r="C15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15">
-        <v>50</v>
-      </c>
-      <c r="F15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16">
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="14">
         <v>52</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F35" s="14" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17">
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+    </row>
+    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="14">
         <v>54</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F36" s="14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18">
-        <v>59</v>
-      </c>
-      <c r="F18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19">
-        <v>61</v>
-      </c>
-      <c r="F19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>73</v>
-      </c>
-      <c r="C20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20">
-        <v>62</v>
-      </c>
-      <c r="F20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E21">
-        <v>63</v>
-      </c>
-      <c r="F21" t="s">
-        <v>84</v>
-      </c>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+    </row>
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="14">
+        <v>18</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>